<commit_message>
Fixed sff9 excel file
</commit_message>
<xml_diff>
--- a/Data/sff3 establishment data.xlsx
+++ b/Data/sff3 establishment data.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Ecology\Student_folders_&amp;_files\Jonathan 2024\sangres_qaqc\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Ecology\Student_folders_&amp;_files\Jonathan 2024\sangres_graphs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169C18CC-F86D-4565-86BA-7162B19557ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846BA3C8-79B9-40F9-A72C-3DFCCAAF5DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$407</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -505,7 +508,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F302" sqref="F302"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7588,20 +7591,12 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D407" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -7613,6 +7608,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7899,14 +7903,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D514523F-DDAE-4B1F-873B-94A8A26807ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51602E44-B4C0-4D8C-A59F-805A7A6C1E2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7914,6 +7910,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9"/>
     <ds:schemaRef ds:uri="31062a0d-ede8-4112-b4bb-00a9c1bc8e16"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D514523F-DDAE-4B1F-873B-94A8A26807ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>